<commit_message>
modified Planning KW3, added Planning KW 5-7
</commit_message>
<xml_diff>
--- a/Planning/KW3.xlsx
+++ b/Planning/KW3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\project-proposal-die_gottlichen_socken\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4882509C-058B-4C46-99A2-58EDC361799D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFAD46D-7095-4C94-A094-F631AEBE2D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{754BBE5A-440E-49BA-984D-71DA240BE7FE}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>

</xml_diff>